<commit_message>
copy updates across to xlsx
</commit_message>
<xml_diff>
--- a/data-raw/su_translations.xlsx
+++ b/data-raw/su_translations.xlsx
@@ -11,7 +11,7 @@
     <sheet name="translations" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="su_translations" vbProcedure="false">translations!$A$1:$D$693</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="su_translations" vbProcedure="false">translations!$A$1:$D$692</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="1724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="1751">
   <si>
     <t xml:space="preserve">@ note: comments are marked with @ and sections are marked with @@</t>
   </si>
@@ -3355,7 +3355,7 @@
     <t xml:space="preserve">Para cada uno de esos atacantes, un desglose por código de ataque (X5, V5, etc) por cada tipo de ataque por el que el jugador haya hecho al menos \\1 ataques</t>
   </si>
   <si>
-    <t xml:space="preserve">Pour chaque attaquant, le detail par codes d'attaques (X5, V5, etc) est donne quand plus de //1 attaques sont enregistrées</t>
+    <t xml:space="preserve">Pour chaque attaquant, le detail par codes d'attaques (X5, V5, etc) est donne quand plus de \\1 attaques sont enregistrées</t>
   </si>
   <si>
     <t xml:space="preserve">Charts/tables are only shown for attack codes (X5, V5, etc) for which the player made at least ([[:digit:]]+) attacks</t>
@@ -3367,7 +3367,7 @@
     <t xml:space="preserve">Diagramas/tablas se muestran solamente para los códigos de ataque (X5, V5, etc) en los que el jugador haya hecho al menos \\1 ataques</t>
   </si>
   <si>
-    <t xml:space="preserve">Les graphiques/tableaux sont seulement proposes pour les codes d'attaques pour lesquels plus de //1 occurences sont enregistrées</t>
+    <t xml:space="preserve">Les graphiques/tableaux sont seulement proposes pour les codes d'attaques pour lesquels plus de \\1 occurences sont enregistrées</t>
   </si>
   <si>
     <t xml:space="preserve">Note that each table below is based on all attacks with the given attack code. However, the charts do not show all attacks</t>
@@ -3649,39 +3649,111 @@
     <t xml:space="preserve">Number of reception attacks by the team when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Número de ataques tras recepción del equipo cuando este jugador estaba en primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de réceptions de l’équipe quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team reception attack kill percentage when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Porcentaje de ataque punto tras recepción del equipo cuando este jugador estaba en primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pourcentage d’attaque gagnantes sur réception de l’équipe quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sideout percentage when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Porcentaje de cambio de saque cuando este jugador estaba primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pourcentage de sideout quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">As for 'N rec att' but only on good or perfect reception</t>
   </si>
   <si>
+    <t xml:space="preserve">Como 'N at rec' pero solo con recepción perfecta o positiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme 'N rec att' mais sur bonne ou excellente réception</t>
+  </si>
+  <si>
     <t xml:space="preserve">As for 'rec att%' but only on good or perfect reception</t>
   </si>
   <si>
+    <t xml:space="preserve">Como '% at rec' pero solo con recepción perfecta o positiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme 'rec att gagn%' mais sur bonne bonne ou excellente réception</t>
+  </si>
+  <si>
     <t xml:space="preserve">As for 'SO%' but only on good or perfect reception</t>
   </si>
   <si>
+    <t xml:space="preserve">Como '% C.S.' pero solo con recepción perfecta o positiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme '%SO' mais sur bonne ou excellente réception</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of transition attacks by the team when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Número de contraataques del equipo cuando este jugador estaba primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre d’attaques en transition de l’équipe quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team transition attack kill percentage when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Porcentaje de contraataque punto cuando este jugador estaba primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poucentage d’attaques gagnantes en transition de l’équipe quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Percentage of points won when a transition attack was made (by any player on the team) and this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Porcentaje de puntos ganados cuando el equipo hizo un contraataque (cualquier jugador) y este jugador estaba primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pourcentage de points gagnés en transition (par n’importe lequel joueur de l’équipe) quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">As for 'N trans att' but only in breakpoint phase (i.e. the team was serving)</t>
   </si>
   <si>
+    <t xml:space="preserve">Como 'N contraat' pero solo en fase breakpoint (cuando el equipo estaba al saque)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme 'N att trans' uniquement sur phase de breakpoint (point gagné sur service)</t>
+  </si>
+  <si>
     <t xml:space="preserve">As for 'trans att%' but only in breakpoint phase (i.e. the team was serving)</t>
   </si>
   <si>
+    <t xml:space="preserve">Como '% contraat' pero solo en fase breakpoint (cuando el equipo estaba al saque)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme 'att trans gagn%' uniquement sur phase de breakpoint (point gagné sur service)</t>
+  </si>
+  <si>
     <t xml:space="preserve">The percentage of points won on serve when this player was front row</t>
   </si>
   <si>
+    <t xml:space="preserve">Porcentaje de puntos ganados al saque cuando este jugador estaba primera línea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pourcentage de points gagnés au service quand ce joueur était devant</t>
+  </si>
+  <si>
     <t xml:space="preserve">@@ blocking section</t>
   </si>
   <si>
@@ -5044,16 +5116,25 @@
     <t xml:space="preserve">Use at your own risk. While every effort has been made to make the reports accurate, no warranty is given and no responsibility is accepted for errors or omissions. Be aware that the outputs from these apps can be affected by errors or inconsistencies in your data, which in general are impossible for the apps to detect or correct. Note also that different scouts use different scouting conventions, and it is not possible to anticipate or cater for all possible variations in these conventions.</t>
   </si>
   <si>
+    <t xml:space="preserve">Utilisez a vos propre risques. Les applications ont été développées avec soin afin de maximiser la qualité du contenu, mais aucune garantie n’est donnée ni aucune responsabilité acceptée en cas d’erreur ou d’omission. Les résultats proposés sont susceptibles d’etre affectées par des erreurs dans vos données, qui sont en général impossibles a détecter par les applications. Par ailleurs, les méthodes de scouting peuvent différer entre scout, et il n’est pas possible d’anticiper toutes les variations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">request_dropbox_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To work with your own data sets, you will need to upload them via Dropbox. Enter your Dropbox email here so that a folder can be shared with you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour travailler avec vos données, vous devez les télécharger via Dropbox. Tapez votre email Dropbox ci-dessous afin de nous permettre de partager un dossier avec vous.</t>
+  </si>
+  <si>
     <t xml:space="preserve">no_app_access</t>
   </si>
   <si>
     <t xml:space="preserve">You do not have access to this application - contact</t>
   </si>
   <si>
-    <t xml:space="preserve">request_dropbox_email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To work with your own data sets, you will need to upload them via Dropbox. Enter your Dropbox email here so that a folder can be shared with you.</t>
+    <t xml:space="preserve">Vous n’avez pas acces a cette application – contact</t>
   </si>
   <si>
     <t xml:space="preserve">@@ progress messages in app</t>
@@ -5194,7 +5275,7 @@
     <t xml:space="preserve">procesando datos</t>
   </si>
   <si>
-    <t xml:space="preserve">des données en traitement</t>
+    <t xml:space="preserve">données en cours de pré-traitement</t>
   </si>
 </sst>
 </file>
@@ -5204,7 +5285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5230,6 +5311,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -5295,11 +5382,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5380,10 +5467,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D694"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A477" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B495" activeCellId="0" sqref="B495"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B440" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D459" activeCellId="0" sqref="D459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11495,2652 +11582,2709 @@
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="3" t="s">
+      <c r="A493" s="1" t="s">
         <v>1207</v>
       </c>
-      <c r="B493" s="4" t="s">
+      <c r="B493" s="1" t="s">
         <v>1207</v>
       </c>
-      <c r="C493" s="3"/>
-      <c r="D493" s="3"/>
+      <c r="C493" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D493" s="1" t="s">
+        <v>1209</v>
+      </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="3" t="s">
-        <v>1208</v>
-      </c>
-      <c r="B494" s="4" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C494" s="3"/>
-      <c r="D494" s="3"/>
+      <c r="A494" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C494" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D494" s="1" t="s">
+        <v>1212</v>
+      </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="3" t="s">
-        <v>1209</v>
-      </c>
-      <c r="B495" s="4" t="s">
-        <v>1209</v>
-      </c>
-      <c r="C495" s="3"/>
-      <c r="D495" s="3"/>
+      <c r="A495" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C495" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D495" s="1" t="s">
+        <v>1215</v>
+      </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="3" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B496" s="4" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C496" s="3"/>
-      <c r="D496" s="3"/>
+      <c r="A496" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C496" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D496" s="1" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="3" t="s">
-        <v>1211</v>
-      </c>
-      <c r="B497" s="4" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C497" s="3"/>
-      <c r="D497" s="3"/>
+      <c r="A497" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C497" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D497" s="1" t="s">
+        <v>1221</v>
+      </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="3" t="s">
-        <v>1212</v>
-      </c>
-      <c r="B498" s="4" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C498" s="3"/>
-      <c r="D498" s="3"/>
+      <c r="A498" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C498" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D498" s="1" t="s">
+        <v>1224</v>
+      </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="3" t="s">
-        <v>1213</v>
-      </c>
-      <c r="B499" s="4" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C499" s="3"/>
-      <c r="D499" s="3"/>
+      <c r="A499" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C499" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D499" s="1" t="s">
+        <v>1227</v>
+      </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="3" t="s">
-        <v>1214</v>
-      </c>
-      <c r="B500" s="4" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C500" s="3"/>
-      <c r="D500" s="3"/>
+      <c r="A500" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C500" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D500" s="1" t="s">
+        <v>1230</v>
+      </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="3" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B501" s="4" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C501" s="3"/>
-      <c r="D501" s="3"/>
+      <c r="A501" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C501" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>1233</v>
+      </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="3" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B502" s="4" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C502" s="3"/>
-      <c r="D502" s="3"/>
+      <c r="A502" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C502" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>1236</v>
+      </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="3" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B503" s="4" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C503" s="3"/>
-      <c r="D503" s="3"/>
+      <c r="A503" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C503" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>1239</v>
+      </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="3" t="s">
-        <v>1218</v>
-      </c>
-      <c r="B504" s="4" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C504" s="3"/>
-      <c r="D504" s="3"/>
+      <c r="A504" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C504" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>1242</v>
+      </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>1219</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>1220</v>
+        <v>1244</v>
       </c>
       <c r="B507" s="0" t="s">
-        <v>1220</v>
+        <v>1244</v>
       </c>
       <c r="C507" s="0" t="s">
-        <v>1221</v>
+        <v>1245</v>
       </c>
       <c r="D507" s="0" t="s">
-        <v>1222</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>1223</v>
+        <v>1247</v>
       </c>
       <c r="B508" s="0" t="s">
-        <v>1223</v>
+        <v>1247</v>
       </c>
       <c r="C508" s="0" t="s">
-        <v>1224</v>
+        <v>1248</v>
       </c>
       <c r="D508" s="0" t="s">
-        <v>1225</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>1226</v>
+        <v>1250</v>
       </c>
       <c r="B509" s="0" t="s">
-        <v>1226</v>
+        <v>1250</v>
       </c>
       <c r="C509" s="0" t="s">
-        <v>1227</v>
+        <v>1251</v>
       </c>
       <c r="D509" s="0" t="s">
-        <v>1228</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>1229</v>
+        <v>1253</v>
       </c>
       <c r="B510" s="0" t="s">
-        <v>1229</v>
+        <v>1253</v>
       </c>
       <c r="C510" s="0" t="s">
-        <v>1229</v>
+        <v>1253</v>
       </c>
       <c r="D510" s="0" t="s">
-        <v>1229</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="0" t="s">
-        <v>1230</v>
+        <v>1254</v>
       </c>
       <c r="B511" s="0" t="s">
-        <v>1230</v>
+        <v>1254</v>
       </c>
       <c r="C511" s="0" t="s">
-        <v>1231</v>
+        <v>1255</v>
       </c>
       <c r="D511" s="0" t="s">
-        <v>1232</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="0" t="s">
-        <v>1233</v>
+        <v>1257</v>
       </c>
       <c r="B512" s="0" t="s">
-        <v>1233</v>
+        <v>1257</v>
       </c>
       <c r="C512" s="0" t="s">
-        <v>1234</v>
+        <v>1258</v>
       </c>
       <c r="D512" s="0" t="s">
-        <v>1233</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>1235</v>
+        <v>1259</v>
       </c>
       <c r="B513" s="0" t="s">
-        <v>1235</v>
+        <v>1259</v>
       </c>
       <c r="C513" s="0" t="s">
-        <v>1236</v>
+        <v>1260</v>
       </c>
       <c r="D513" s="0" t="s">
-        <v>1237</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="0" t="s">
-        <v>1238</v>
+        <v>1262</v>
       </c>
       <c r="B514" s="0" t="s">
-        <v>1238</v>
+        <v>1262</v>
       </c>
       <c r="C514" s="0" t="s">
-        <v>1239</v>
+        <v>1263</v>
       </c>
       <c r="D514" s="0" t="s">
-        <v>1238</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>1240</v>
+        <v>1264</v>
       </c>
       <c r="B515" s="0" t="s">
-        <v>1240</v>
+        <v>1264</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>1241</v>
+        <v>1265</v>
       </c>
       <c r="D515" s="0" t="s">
-        <v>1242</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
-        <v>1243</v>
+        <v>1267</v>
       </c>
       <c r="B516" s="0" t="s">
-        <v>1243</v>
+        <v>1267</v>
       </c>
       <c r="C516" s="0" t="s">
-        <v>1244</v>
+        <v>1268</v>
       </c>
       <c r="D516" s="0" t="s">
-        <v>1245</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="0" t="s">
-        <v>1246</v>
+        <v>1270</v>
       </c>
       <c r="B517" s="0" t="s">
-        <v>1246</v>
+        <v>1270</v>
       </c>
       <c r="C517" s="0" t="s">
-        <v>1247</v>
+        <v>1271</v>
       </c>
       <c r="D517" s="0" t="s">
-        <v>1248</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="0" t="s">
-        <v>1249</v>
+        <v>1273</v>
       </c>
       <c r="B518" s="0" t="s">
-        <v>1249</v>
+        <v>1273</v>
       </c>
       <c r="C518" s="0" t="s">
-        <v>1250</v>
+        <v>1274</v>
       </c>
       <c r="D518" s="0" t="s">
-        <v>1251</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>1252</v>
+        <v>1276</v>
       </c>
       <c r="B519" s="0" t="s">
-        <v>1252</v>
+        <v>1276</v>
       </c>
       <c r="C519" s="0" t="s">
-        <v>1252</v>
+        <v>1276</v>
       </c>
       <c r="D519" s="0" t="s">
-        <v>1253</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>1254</v>
+        <v>1278</v>
       </c>
       <c r="B520" s="0" t="s">
-        <v>1254</v>
+        <v>1278</v>
       </c>
       <c r="C520" s="0" t="s">
-        <v>1254</v>
+        <v>1278</v>
       </c>
       <c r="D520" s="0" t="s">
-        <v>1255</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>1256</v>
+        <v>1280</v>
       </c>
       <c r="B521" s="0" t="s">
-        <v>1256</v>
+        <v>1280</v>
       </c>
       <c r="C521" s="0" t="s">
-        <v>1257</v>
+        <v>1281</v>
       </c>
       <c r="D521" s="0" t="s">
-        <v>1258</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>1259</v>
+        <v>1283</v>
       </c>
       <c r="B522" s="0" t="s">
-        <v>1259</v>
+        <v>1283</v>
       </c>
       <c r="C522" s="0" t="s">
-        <v>1260</v>
+        <v>1284</v>
       </c>
       <c r="D522" s="0" t="s">
-        <v>1259</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="0" t="s">
-        <v>1261</v>
+        <v>1285</v>
       </c>
       <c r="B523" s="0" t="s">
-        <v>1261</v>
+        <v>1285</v>
       </c>
       <c r="C523" s="0" t="s">
-        <v>1262</v>
+        <v>1286</v>
       </c>
       <c r="D523" s="0" t="s">
-        <v>1263</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="0" t="s">
-        <v>1264</v>
+        <v>1288</v>
       </c>
       <c r="B524" s="0" t="s">
-        <v>1264</v>
+        <v>1288</v>
       </c>
       <c r="C524" s="0" t="s">
-        <v>1265</v>
+        <v>1289</v>
       </c>
       <c r="D524" s="0" t="s">
-        <v>1266</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="0" t="s">
-        <v>1267</v>
+        <v>1291</v>
       </c>
       <c r="B525" s="0" t="s">
-        <v>1267</v>
+        <v>1291</v>
       </c>
       <c r="C525" s="0" t="s">
-        <v>1267</v>
+        <v>1291</v>
       </c>
       <c r="D525" s="0" t="s">
-        <v>1267</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="0" t="s">
-        <v>1268</v>
+        <v>1292</v>
       </c>
       <c r="B526" s="0" t="s">
-        <v>1268</v>
+        <v>1292</v>
       </c>
       <c r="C526" s="0" t="s">
-        <v>1269</v>
+        <v>1293</v>
       </c>
       <c r="D526" s="0" t="s">
-        <v>1270</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="0" t="s">
-        <v>1271</v>
+        <v>1295</v>
       </c>
       <c r="B527" s="0" t="s">
-        <v>1271</v>
+        <v>1295</v>
       </c>
       <c r="C527" s="0" t="s">
-        <v>1272</v>
+        <v>1296</v>
       </c>
       <c r="D527" s="0" t="s">
-        <v>1273</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="0" t="s">
-        <v>1274</v>
+        <v>1298</v>
       </c>
       <c r="B528" s="0" t="s">
-        <v>1274</v>
+        <v>1298</v>
       </c>
       <c r="C528" s="0" t="s">
-        <v>1275</v>
+        <v>1299</v>
       </c>
       <c r="D528" s="0" t="s">
-        <v>1276</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="0" t="s">
-        <v>1277</v>
+        <v>1301</v>
       </c>
       <c r="B529" s="0" t="s">
-        <v>1277</v>
+        <v>1301</v>
       </c>
       <c r="C529" s="0" t="s">
-        <v>1278</v>
+        <v>1302</v>
       </c>
       <c r="D529" s="0" t="s">
-        <v>1279</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>1280</v>
+        <v>1304</v>
       </c>
       <c r="B530" s="0" t="s">
-        <v>1280</v>
+        <v>1304</v>
       </c>
       <c r="C530" s="0" t="s">
-        <v>1281</v>
+        <v>1305</v>
       </c>
       <c r="D530" s="0" t="s">
-        <v>1282</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>1283</v>
+        <v>1307</v>
       </c>
       <c r="B531" s="0" t="s">
-        <v>1283</v>
+        <v>1307</v>
       </c>
       <c r="C531" s="0" t="s">
-        <v>1283</v>
+        <v>1307</v>
       </c>
       <c r="D531" s="0" t="s">
-        <v>1283</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>1284</v>
+        <v>1308</v>
       </c>
       <c r="B532" s="0" t="s">
-        <v>1284</v>
+        <v>1308</v>
       </c>
       <c r="C532" s="0" t="s">
-        <v>1285</v>
+        <v>1309</v>
       </c>
       <c r="D532" s="0" t="s">
-        <v>1286</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>1287</v>
+        <v>1311</v>
       </c>
       <c r="B533" s="0" t="s">
-        <v>1287</v>
+        <v>1311</v>
       </c>
       <c r="C533" s="0" t="s">
-        <v>1287</v>
+        <v>1311</v>
       </c>
       <c r="D533" s="0" t="s">
-        <v>1287</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>1288</v>
+        <v>1312</v>
       </c>
       <c r="B534" s="0" t="s">
-        <v>1288</v>
+        <v>1312</v>
       </c>
       <c r="C534" s="0" t="s">
-        <v>1289</v>
+        <v>1313</v>
       </c>
       <c r="D534" s="0" t="s">
-        <v>1290</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>1291</v>
+        <v>1315</v>
       </c>
       <c r="B535" s="0" t="s">
-        <v>1291</v>
+        <v>1315</v>
       </c>
       <c r="C535" s="0" t="s">
-        <v>1292</v>
+        <v>1316</v>
       </c>
       <c r="D535" s="0" t="s">
-        <v>1291</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>1293</v>
+        <v>1317</v>
       </c>
       <c r="B536" s="0" t="s">
-        <v>1293</v>
+        <v>1317</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>1294</v>
+        <v>1318</v>
       </c>
       <c r="D536" s="0" t="s">
-        <v>1295</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>1296</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="0" t="s">
-        <v>1297</v>
+        <v>1321</v>
       </c>
       <c r="B538" s="0" t="s">
-        <v>1297</v>
+        <v>1321</v>
       </c>
       <c r="C538" s="0" t="s">
-        <v>1298</v>
+        <v>1322</v>
       </c>
       <c r="D538" s="0" t="s">
-        <v>1297</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="0" t="s">
-        <v>1299</v>
+        <v>1323</v>
       </c>
       <c r="B539" s="0" t="s">
-        <v>1299</v>
+        <v>1323</v>
       </c>
       <c r="C539" s="0" t="s">
-        <v>1300</v>
+        <v>1324</v>
       </c>
       <c r="D539" s="0" t="s">
-        <v>1301</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="0" t="s">
-        <v>1302</v>
+        <v>1326</v>
       </c>
       <c r="B540" s="0" t="s">
-        <v>1302</v>
+        <v>1326</v>
       </c>
       <c r="C540" s="0" t="s">
-        <v>1303</v>
+        <v>1327</v>
       </c>
       <c r="D540" s="0" t="s">
-        <v>1304</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>1305</v>
+        <v>1329</v>
       </c>
       <c r="B541" s="0" t="s">
-        <v>1305</v>
+        <v>1329</v>
       </c>
       <c r="C541" s="0" t="s">
-        <v>1306</v>
+        <v>1330</v>
       </c>
       <c r="D541" s="0" t="s">
-        <v>1307</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="0" t="s">
-        <v>1308</v>
+        <v>1332</v>
       </c>
       <c r="B542" s="0" t="s">
-        <v>1308</v>
+        <v>1332</v>
       </c>
       <c r="C542" s="0" t="s">
-        <v>1309</v>
+        <v>1333</v>
       </c>
       <c r="D542" s="0" t="s">
-        <v>1308</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="0" t="s">
-        <v>1310</v>
+        <v>1334</v>
       </c>
       <c r="B543" s="0" t="s">
-        <v>1310</v>
+        <v>1334</v>
       </c>
       <c r="C543" s="0" t="s">
-        <v>1311</v>
+        <v>1335</v>
       </c>
       <c r="D543" s="0" t="s">
-        <v>1310</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>1312</v>
+        <v>1336</v>
       </c>
       <c r="B544" s="0" t="s">
-        <v>1312</v>
+        <v>1336</v>
       </c>
       <c r="C544" s="0" t="s">
-        <v>1313</v>
+        <v>1337</v>
       </c>
       <c r="D544" s="0" t="s">
-        <v>1312</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="0" t="s">
-        <v>1314</v>
+        <v>1338</v>
       </c>
       <c r="B545" s="0" t="s">
-        <v>1314</v>
+        <v>1338</v>
       </c>
       <c r="C545" s="0" t="s">
-        <v>1315</v>
+        <v>1339</v>
       </c>
       <c r="D545" s="0" t="s">
-        <v>1314</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="0" t="s">
-        <v>1316</v>
+        <v>1340</v>
       </c>
       <c r="B546" s="0" t="s">
-        <v>1316</v>
+        <v>1340</v>
       </c>
       <c r="C546" s="0" t="s">
-        <v>1317</v>
+        <v>1341</v>
       </c>
       <c r="D546" s="0" t="s">
-        <v>1318</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="0" t="s">
-        <v>1319</v>
+        <v>1343</v>
       </c>
       <c r="B547" s="0" t="s">
-        <v>1319</v>
+        <v>1343</v>
       </c>
       <c r="C547" s="0" t="s">
-        <v>1320</v>
+        <v>1344</v>
       </c>
       <c r="D547" s="0" t="s">
-        <v>1321</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="0" t="s">
-        <v>1322</v>
+        <v>1346</v>
       </c>
       <c r="B548" s="0" t="s">
-        <v>1322</v>
+        <v>1346</v>
       </c>
       <c r="C548" s="0" t="s">
-        <v>1323</v>
+        <v>1347</v>
       </c>
       <c r="D548" s="0" t="s">
-        <v>1324</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="0" t="s">
-        <v>1325</v>
+        <v>1349</v>
       </c>
       <c r="B549" s="0" t="s">
-        <v>1325</v>
+        <v>1349</v>
       </c>
       <c r="C549" s="0" t="s">
-        <v>1326</v>
+        <v>1350</v>
       </c>
       <c r="D549" s="0" t="s">
-        <v>1327</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="0" t="s">
-        <v>1328</v>
+        <v>1352</v>
       </c>
       <c r="B550" s="0" t="s">
-        <v>1328</v>
+        <v>1352</v>
       </c>
       <c r="C550" s="0" t="s">
-        <v>1329</v>
+        <v>1353</v>
       </c>
       <c r="D550" s="0" t="s">
-        <v>1330</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>1331</v>
+        <v>1355</v>
       </c>
       <c r="B551" s="0" t="s">
-        <v>1331</v>
+        <v>1355</v>
       </c>
       <c r="C551" s="0" t="s">
-        <v>1332</v>
+        <v>1356</v>
       </c>
       <c r="D551" s="0" t="s">
-        <v>1333</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="0" t="s">
-        <v>1334</v>
+        <v>1358</v>
       </c>
       <c r="B552" s="0" t="s">
-        <v>1334</v>
+        <v>1358</v>
       </c>
       <c r="C552" s="0" t="s">
-        <v>1334</v>
+        <v>1358</v>
       </c>
       <c r="D552" s="0" t="s">
-        <v>1335</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="0" t="s">
-        <v>1336</v>
+        <v>1360</v>
       </c>
       <c r="B553" s="0" t="s">
-        <v>1336</v>
+        <v>1360</v>
       </c>
       <c r="C553" s="0" t="s">
-        <v>1337</v>
+        <v>1361</v>
       </c>
       <c r="D553" s="0" t="s">
-        <v>1338</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>1339</v>
+        <v>1363</v>
       </c>
       <c r="B554" s="0" t="s">
-        <v>1339</v>
+        <v>1363</v>
       </c>
       <c r="C554" s="0" t="s">
-        <v>1236</v>
+        <v>1260</v>
       </c>
       <c r="D554" s="0" t="s">
-        <v>1340</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>1341</v>
+        <v>1365</v>
       </c>
       <c r="B555" s="0" t="s">
-        <v>1341</v>
+        <v>1365</v>
       </c>
       <c r="C555" s="0" t="s">
-        <v>1342</v>
+        <v>1366</v>
       </c>
       <c r="D555" s="0" t="s">
-        <v>1343</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="0" t="s">
-        <v>1344</v>
+        <v>1368</v>
       </c>
       <c r="B556" s="0" t="s">
-        <v>1344</v>
+        <v>1368</v>
       </c>
       <c r="C556" s="0" t="s">
-        <v>1345</v>
+        <v>1369</v>
       </c>
       <c r="D556" s="0" t="s">
-        <v>1346</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="0" t="s">
-        <v>1347</v>
+        <v>1371</v>
       </c>
       <c r="B557" s="0" t="s">
-        <v>1347</v>
+        <v>1371</v>
       </c>
       <c r="C557" s="0" t="s">
-        <v>1347</v>
+        <v>1371</v>
       </c>
       <c r="D557" s="0" t="s">
-        <v>1348</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="0" t="s">
-        <v>1349</v>
+        <v>1373</v>
       </c>
       <c r="B558" s="0" t="s">
-        <v>1349</v>
+        <v>1373</v>
       </c>
       <c r="C558" s="0" t="s">
-        <v>1350</v>
+        <v>1374</v>
       </c>
       <c r="D558" s="0" t="s">
-        <v>1351</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="0" t="s">
-        <v>1352</v>
+        <v>1376</v>
       </c>
       <c r="B559" s="0" t="s">
-        <v>1352</v>
+        <v>1376</v>
       </c>
       <c r="C559" s="0" t="s">
-        <v>1353</v>
+        <v>1377</v>
       </c>
       <c r="D559" s="0" t="s">
-        <v>1354</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="0" t="s">
-        <v>1355</v>
+        <v>1379</v>
       </c>
       <c r="B560" s="0" t="s">
-        <v>1355</v>
+        <v>1379</v>
       </c>
       <c r="C560" s="0" t="s">
-        <v>1355</v>
+        <v>1379</v>
       </c>
       <c r="D560" s="0" t="s">
-        <v>1355</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="0" t="s">
-        <v>1356</v>
+        <v>1380</v>
       </c>
       <c r="B561" s="0" t="s">
-        <v>1356</v>
+        <v>1380</v>
       </c>
       <c r="C561" s="0" t="s">
-        <v>1356</v>
+        <v>1380</v>
       </c>
       <c r="D561" s="0" t="s">
-        <v>1356</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="0" t="s">
-        <v>1357</v>
+        <v>1381</v>
       </c>
       <c r="B562" s="0" t="s">
-        <v>1357</v>
+        <v>1381</v>
       </c>
       <c r="C562" s="0" t="s">
-        <v>1357</v>
+        <v>1381</v>
       </c>
       <c r="D562" s="0" t="s">
-        <v>1357</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="0" t="s">
-        <v>1358</v>
+        <v>1382</v>
       </c>
       <c r="B563" s="0" t="s">
-        <v>1358</v>
+        <v>1382</v>
       </c>
       <c r="C563" s="0" t="s">
-        <v>1358</v>
+        <v>1382</v>
       </c>
       <c r="D563" s="0" t="s">
-        <v>1358</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="0" t="s">
-        <v>1359</v>
+        <v>1383</v>
       </c>
       <c r="B564" s="0" t="s">
-        <v>1359</v>
+        <v>1383</v>
       </c>
       <c r="C564" s="0" t="s">
-        <v>1360</v>
+        <v>1384</v>
       </c>
       <c r="D564" s="0" t="s">
-        <v>1361</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="0" t="s">
-        <v>1362</v>
+        <v>1386</v>
       </c>
       <c r="B565" s="0" t="s">
-        <v>1362</v>
+        <v>1386</v>
       </c>
       <c r="C565" s="0" t="s">
-        <v>1363</v>
+        <v>1387</v>
       </c>
       <c r="D565" s="0" t="s">
-        <v>1362</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="0" t="s">
-        <v>1364</v>
+        <v>1388</v>
       </c>
       <c r="B566" s="0" t="s">
-        <v>1364</v>
+        <v>1388</v>
       </c>
       <c r="C566" s="0" t="s">
-        <v>1365</v>
+        <v>1389</v>
       </c>
       <c r="D566" s="0" t="s">
-        <v>1366</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="0" t="s">
-        <v>1367</v>
+        <v>1391</v>
       </c>
       <c r="B567" s="0" t="s">
-        <v>1367</v>
+        <v>1391</v>
       </c>
       <c r="C567" s="0" t="s">
-        <v>1368</v>
+        <v>1392</v>
       </c>
       <c r="D567" s="0" t="s">
-        <v>1367</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="0" t="s">
-        <v>1369</v>
+        <v>1393</v>
       </c>
       <c r="B568" s="0" t="s">
-        <v>1369</v>
+        <v>1393</v>
       </c>
       <c r="C568" s="0" t="s">
-        <v>1370</v>
+        <v>1394</v>
       </c>
       <c r="D568" s="0" t="s">
-        <v>1237</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="0" t="s">
-        <v>1371</v>
+        <v>1395</v>
       </c>
       <c r="B569" s="0" t="s">
-        <v>1371</v>
+        <v>1395</v>
       </c>
       <c r="C569" s="0" t="s">
-        <v>1372</v>
+        <v>1396</v>
       </c>
       <c r="D569" s="0" t="s">
-        <v>1373</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="0" t="s">
-        <v>1374</v>
+        <v>1398</v>
       </c>
       <c r="B570" s="0" t="s">
-        <v>1374</v>
+        <v>1398</v>
       </c>
       <c r="C570" s="0" t="s">
-        <v>1375</v>
+        <v>1399</v>
       </c>
       <c r="D570" s="0" t="s">
-        <v>1376</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="0" t="s">
-        <v>1377</v>
+        <v>1401</v>
       </c>
       <c r="B571" s="0" t="s">
-        <v>1377</v>
+        <v>1401</v>
       </c>
       <c r="C571" s="0" t="s">
-        <v>1378</v>
+        <v>1402</v>
       </c>
       <c r="D571" s="0" t="s">
-        <v>1379</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="0" t="s">
-        <v>1380</v>
+        <v>1404</v>
       </c>
       <c r="B572" s="0" t="s">
-        <v>1380</v>
+        <v>1404</v>
       </c>
       <c r="C572" s="0" t="s">
-        <v>1381</v>
+        <v>1405</v>
       </c>
       <c r="D572" s="0" t="s">
-        <v>1382</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="0" t="s">
-        <v>1383</v>
+        <v>1407</v>
       </c>
       <c r="B573" s="0" t="s">
-        <v>1383</v>
+        <v>1407</v>
       </c>
       <c r="C573" s="0" t="s">
-        <v>1384</v>
+        <v>1408</v>
       </c>
       <c r="D573" s="0" t="s">
-        <v>1385</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="0" t="s">
-        <v>1386</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="0" t="s">
-        <v>1387</v>
+        <v>1411</v>
       </c>
       <c r="B576" s="0" t="s">
-        <v>1387</v>
+        <v>1411</v>
       </c>
       <c r="C576" s="0" t="s">
-        <v>1388</v>
+        <v>1412</v>
       </c>
       <c r="D576" s="0" t="s">
-        <v>1389</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="0" t="s">
-        <v>1390</v>
+        <v>1414</v>
       </c>
       <c r="B577" s="0" t="s">
-        <v>1390</v>
+        <v>1414</v>
       </c>
       <c r="C577" s="0" t="s">
-        <v>1391</v>
+        <v>1415</v>
       </c>
       <c r="D577" s="0" t="s">
-        <v>1392</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="0" t="s">
-        <v>1393</v>
+        <v>1417</v>
       </c>
       <c r="B578" s="0" t="s">
-        <v>1393</v>
+        <v>1417</v>
       </c>
       <c r="C578" s="0" t="s">
-        <v>1394</v>
+        <v>1418</v>
       </c>
       <c r="D578" s="0" t="s">
-        <v>1395</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="0" t="s">
-        <v>1396</v>
+        <v>1420</v>
       </c>
       <c r="B579" s="0" t="s">
-        <v>1396</v>
+        <v>1420</v>
       </c>
       <c r="C579" s="0" t="s">
-        <v>1397</v>
+        <v>1421</v>
       </c>
       <c r="D579" s="0" t="s">
-        <v>1398</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="0" t="s">
-        <v>1399</v>
+        <v>1423</v>
       </c>
       <c r="B580" s="0" t="s">
-        <v>1399</v>
+        <v>1423</v>
       </c>
       <c r="C580" s="0" t="s">
-        <v>1400</v>
+        <v>1424</v>
       </c>
       <c r="D580" s="0" t="s">
-        <v>1401</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="0" t="s">
-        <v>1402</v>
+        <v>1426</v>
       </c>
       <c r="B581" s="0" t="s">
-        <v>1402</v>
+        <v>1426</v>
       </c>
       <c r="C581" s="0" t="s">
-        <v>1403</v>
+        <v>1427</v>
       </c>
       <c r="D581" s="0" t="s">
-        <v>1401</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="0" t="s">
-        <v>1404</v>
+        <v>1428</v>
       </c>
       <c r="B582" s="0" t="s">
-        <v>1404</v>
+        <v>1428</v>
       </c>
       <c r="C582" s="0" t="s">
-        <v>1405</v>
+        <v>1429</v>
       </c>
       <c r="D582" s="0" t="s">
-        <v>1406</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="0" t="s">
-        <v>1407</v>
+        <v>1431</v>
       </c>
       <c r="B583" s="0" t="s">
-        <v>1407</v>
+        <v>1431</v>
       </c>
       <c r="C583" s="0" t="s">
-        <v>1408</v>
+        <v>1432</v>
       </c>
       <c r="D583" s="0" t="s">
-        <v>1409</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="0" t="s">
-        <v>1410</v>
+        <v>1434</v>
       </c>
       <c r="B584" s="0" t="s">
-        <v>1410</v>
+        <v>1434</v>
       </c>
       <c r="C584" s="0" t="s">
-        <v>1411</v>
+        <v>1435</v>
       </c>
       <c r="D584" s="0" t="s">
-        <v>1412</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="0" t="s">
-        <v>1413</v>
+        <v>1437</v>
       </c>
       <c r="B585" s="0" t="s">
-        <v>1413</v>
+        <v>1437</v>
       </c>
       <c r="C585" s="0" t="s">
-        <v>1414</v>
+        <v>1438</v>
       </c>
       <c r="D585" s="0" t="s">
-        <v>1415</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="0" t="s">
-        <v>1416</v>
+        <v>1440</v>
       </c>
       <c r="B586" s="0" t="s">
-        <v>1416</v>
+        <v>1440</v>
       </c>
       <c r="C586" s="0" t="s">
-        <v>1417</v>
+        <v>1441</v>
       </c>
       <c r="D586" s="0" t="s">
-        <v>1418</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="0" t="s">
-        <v>1419</v>
+        <v>1443</v>
       </c>
       <c r="B587" s="0" t="s">
-        <v>1419</v>
+        <v>1443</v>
       </c>
       <c r="C587" s="0" t="s">
-        <v>1420</v>
+        <v>1444</v>
       </c>
       <c r="D587" s="0" t="s">
-        <v>1421</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>1422</v>
+        <v>1446</v>
       </c>
       <c r="B588" s="0" t="s">
-        <v>1422</v>
+        <v>1446</v>
       </c>
       <c r="C588" s="0" t="s">
-        <v>1423</v>
+        <v>1447</v>
       </c>
       <c r="D588" s="0" t="s">
-        <v>1424</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>1425</v>
+        <v>1449</v>
       </c>
       <c r="B589" s="0" t="s">
-        <v>1425</v>
+        <v>1449</v>
       </c>
       <c r="C589" s="0" t="s">
-        <v>1426</v>
+        <v>1450</v>
       </c>
       <c r="D589" s="0" t="s">
-        <v>1427</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="0" t="s">
-        <v>1428</v>
+        <v>1452</v>
       </c>
       <c r="B590" s="0" t="s">
-        <v>1428</v>
+        <v>1452</v>
       </c>
       <c r="C590" s="0" t="s">
-        <v>1429</v>
+        <v>1453</v>
       </c>
       <c r="D590" s="0" t="s">
-        <v>1430</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="0" t="s">
-        <v>1431</v>
+        <v>1455</v>
       </c>
       <c r="B591" s="0" t="s">
-        <v>1431</v>
+        <v>1455</v>
       </c>
       <c r="C591" s="0" t="s">
-        <v>1432</v>
+        <v>1456</v>
       </c>
       <c r="D591" s="0" t="s">
-        <v>1433</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>1434</v>
+        <v>1458</v>
       </c>
       <c r="B592" s="0" t="s">
-        <v>1434</v>
+        <v>1458</v>
       </c>
       <c r="C592" s="0" t="s">
-        <v>1435</v>
+        <v>1459</v>
       </c>
       <c r="D592" s="0" t="s">
-        <v>1436</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
-        <v>1437</v>
+        <v>1461</v>
       </c>
       <c r="B593" s="0" t="s">
-        <v>1437</v>
+        <v>1461</v>
       </c>
       <c r="C593" s="0" t="s">
-        <v>1438</v>
+        <v>1462</v>
       </c>
       <c r="D593" s="0" t="s">
-        <v>1439</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="594" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="0" t="s">
-        <v>1440</v>
+        <v>1464</v>
       </c>
       <c r="B594" s="0" t="s">
-        <v>1440</v>
+        <v>1464</v>
       </c>
       <c r="C594" s="0" t="s">
-        <v>1441</v>
+        <v>1465</v>
       </c>
       <c r="D594" s="0" t="s">
-        <v>1442</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="0" t="s">
-        <v>1443</v>
+        <v>1467</v>
       </c>
       <c r="B595" s="0" t="s">
-        <v>1443</v>
+        <v>1467</v>
       </c>
       <c r="C595" s="0" t="s">
-        <v>1444</v>
+        <v>1468</v>
       </c>
       <c r="D595" s="0" t="s">
-        <v>1445</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="0" t="s">
-        <v>1446</v>
+        <v>1470</v>
       </c>
       <c r="B596" s="0" t="s">
-        <v>1446</v>
+        <v>1470</v>
       </c>
       <c r="C596" s="0" t="s">
-        <v>1447</v>
+        <v>1471</v>
       </c>
       <c r="D596" s="0" t="s">
-        <v>1448</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="0" t="s">
-        <v>1449</v>
+        <v>1473</v>
       </c>
       <c r="B597" s="0" t="s">
-        <v>1449</v>
+        <v>1473</v>
       </c>
       <c r="C597" s="0" t="s">
-        <v>1450</v>
+        <v>1474</v>
       </c>
       <c r="D597" s="0" t="s">
-        <v>1451</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="0" t="s">
-        <v>1452</v>
+        <v>1476</v>
       </c>
       <c r="B598" s="0" t="s">
-        <v>1452</v>
+        <v>1476</v>
       </c>
       <c r="C598" s="0" t="s">
-        <v>1453</v>
+        <v>1477</v>
       </c>
       <c r="D598" s="0" t="s">
-        <v>1454</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="0" t="s">
-        <v>1455</v>
+        <v>1479</v>
       </c>
       <c r="B599" s="0" t="s">
-        <v>1455</v>
+        <v>1479</v>
       </c>
       <c r="C599" s="0" t="s">
-        <v>1456</v>
+        <v>1480</v>
       </c>
       <c r="D599" s="0" t="s">
-        <v>1457</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="0" t="s">
-        <v>1458</v>
+        <v>1482</v>
       </c>
       <c r="B600" s="0" t="s">
-        <v>1458</v>
+        <v>1482</v>
       </c>
       <c r="C600" s="0" t="s">
-        <v>1459</v>
+        <v>1483</v>
       </c>
       <c r="D600" s="0" t="s">
-        <v>1460</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="0" t="s">
-        <v>1461</v>
+        <v>1485</v>
       </c>
       <c r="B601" s="0" t="s">
-        <v>1461</v>
+        <v>1485</v>
       </c>
       <c r="C601" s="0" t="s">
-        <v>1462</v>
+        <v>1486</v>
       </c>
       <c r="D601" s="0" t="s">
-        <v>1463</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="0" t="s">
-        <v>1464</v>
+        <v>1488</v>
       </c>
       <c r="B602" s="0" t="s">
-        <v>1464</v>
+        <v>1488</v>
       </c>
       <c r="C602" s="0" t="s">
-        <v>1465</v>
+        <v>1489</v>
       </c>
       <c r="D602" s="0" t="s">
-        <v>1466</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="0" t="s">
-        <v>1467</v>
+        <v>1491</v>
       </c>
       <c r="B603" s="0" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C603" s="3" t="s">
-        <v>1468</v>
+        <v>1491</v>
+      </c>
+      <c r="C603" s="4" t="s">
+        <v>1492</v>
       </c>
       <c r="D603" s="0" t="s">
-        <v>1469</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="0" t="s">
-        <v>1470</v>
+        <v>1494</v>
       </c>
       <c r="B604" s="0" t="s">
-        <v>1470</v>
+        <v>1494</v>
       </c>
       <c r="C604" s="0" t="s">
-        <v>1471</v>
+        <v>1495</v>
       </c>
       <c r="D604" s="0" t="s">
-        <v>1472</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="0" t="s">
-        <v>1473</v>
+        <v>1497</v>
       </c>
       <c r="B605" s="0" t="s">
-        <v>1473</v>
+        <v>1497</v>
       </c>
       <c r="C605" s="1" t="s">
-        <v>1474</v>
+        <v>1498</v>
       </c>
       <c r="D605" s="0" t="s">
-        <v>1475</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="0" t="s">
-        <v>1476</v>
+        <v>1500</v>
       </c>
       <c r="B606" s="0" t="s">
-        <v>1476</v>
+        <v>1500</v>
       </c>
       <c r="C606" s="0" t="s">
-        <v>1477</v>
+        <v>1501</v>
       </c>
       <c r="D606" s="0" t="s">
-        <v>1478</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="0" t="s">
-        <v>1479</v>
+        <v>1503</v>
       </c>
       <c r="B607" s="0" t="s">
-        <v>1479</v>
+        <v>1503</v>
       </c>
       <c r="C607" s="0" t="s">
-        <v>1480</v>
+        <v>1504</v>
       </c>
       <c r="D607" s="0" t="s">
-        <v>1481</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
-        <v>1482</v>
+        <v>1506</v>
       </c>
       <c r="B608" s="0" t="s">
-        <v>1482</v>
+        <v>1506</v>
       </c>
       <c r="C608" s="0" t="s">
-        <v>1483</v>
+        <v>1507</v>
       </c>
       <c r="D608" s="0" t="s">
-        <v>1484</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="0" t="s">
-        <v>1485</v>
+        <v>1509</v>
       </c>
       <c r="B609" s="0" t="s">
-        <v>1485</v>
+        <v>1509</v>
       </c>
       <c r="C609" s="0" t="s">
-        <v>1486</v>
+        <v>1510</v>
       </c>
       <c r="D609" s="0" t="s">
-        <v>1487</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="0" t="s">
-        <v>1488</v>
+        <v>1512</v>
       </c>
       <c r="B610" s="0" t="s">
-        <v>1488</v>
+        <v>1512</v>
       </c>
       <c r="C610" s="0" t="s">
-        <v>1489</v>
+        <v>1513</v>
       </c>
       <c r="D610" s="0" t="s">
-        <v>1490</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="0" t="s">
-        <v>1491</v>
+        <v>1515</v>
       </c>
       <c r="B611" s="0" t="s">
-        <v>1491</v>
+        <v>1515</v>
       </c>
       <c r="C611" s="0" t="s">
-        <v>1492</v>
+        <v>1516</v>
       </c>
       <c r="D611" s="0" t="s">
-        <v>1493</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="0" t="s">
-        <v>1494</v>
+        <v>1518</v>
       </c>
       <c r="B612" s="0" t="s">
-        <v>1494</v>
+        <v>1518</v>
       </c>
       <c r="C612" s="0" t="s">
-        <v>1495</v>
+        <v>1519</v>
       </c>
       <c r="D612" s="0" t="s">
-        <v>1496</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="0" t="s">
-        <v>1497</v>
+        <v>1521</v>
       </c>
       <c r="B613" s="0" t="s">
-        <v>1497</v>
+        <v>1521</v>
       </c>
       <c r="C613" s="0" t="s">
-        <v>1498</v>
+        <v>1522</v>
       </c>
       <c r="D613" s="0" t="s">
-        <v>1497</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="0" t="s">
-        <v>1499</v>
+        <v>1523</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>1499</v>
+        <v>1523</v>
       </c>
       <c r="C614" s="0" t="s">
-        <v>1500</v>
+        <v>1524</v>
       </c>
       <c r="D614" s="0" t="s">
-        <v>1501</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="0" t="s">
-        <v>1502</v>
+        <v>1526</v>
       </c>
       <c r="B615" s="0" t="s">
-        <v>1502</v>
+        <v>1526</v>
       </c>
       <c r="C615" s="0" t="s">
-        <v>1503</v>
+        <v>1527</v>
       </c>
       <c r="D615" s="0" t="s">
-        <v>1504</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="0" t="s">
-        <v>1505</v>
+        <v>1529</v>
       </c>
       <c r="B616" s="0" t="s">
-        <v>1505</v>
+        <v>1529</v>
       </c>
       <c r="C616" s="0" t="s">
-        <v>1506</v>
+        <v>1530</v>
       </c>
       <c r="D616" s="0" t="s">
-        <v>1507</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="0" t="s">
-        <v>1508</v>
+        <v>1532</v>
       </c>
       <c r="B617" s="0" t="s">
-        <v>1508</v>
+        <v>1532</v>
       </c>
       <c r="C617" s="0" t="s">
-        <v>1509</v>
+        <v>1533</v>
       </c>
       <c r="D617" s="0" t="s">
-        <v>1510</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="0" t="s">
-        <v>1511</v>
+        <v>1535</v>
       </c>
       <c r="B618" s="0" t="s">
-        <v>1511</v>
+        <v>1535</v>
       </c>
       <c r="C618" s="0" t="s">
-        <v>1512</v>
+        <v>1536</v>
       </c>
       <c r="D618" s="0" t="s">
-        <v>1513</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="0" t="s">
-        <v>1514</v>
+        <v>1538</v>
       </c>
       <c r="B619" s="0" t="s">
-        <v>1514</v>
+        <v>1538</v>
       </c>
       <c r="C619" s="0" t="s">
-        <v>1515</v>
+        <v>1539</v>
       </c>
       <c r="D619" s="0" t="s">
-        <v>1516</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="0" t="s">
-        <v>1517</v>
+        <v>1541</v>
       </c>
       <c r="B620" s="0" t="s">
-        <v>1517</v>
+        <v>1541</v>
       </c>
       <c r="C620" s="0" t="s">
-        <v>1518</v>
+        <v>1542</v>
       </c>
       <c r="D620" s="0" t="s">
-        <v>1519</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="0" t="s">
-        <v>1520</v>
+        <v>1544</v>
       </c>
       <c r="B621" s="0" t="s">
-        <v>1520</v>
+        <v>1544</v>
       </c>
       <c r="C621" s="0" t="s">
-        <v>1521</v>
+        <v>1545</v>
       </c>
       <c r="D621" s="0" t="s">
-        <v>1522</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="0" t="s">
-        <v>1523</v>
+        <v>1547</v>
       </c>
       <c r="B622" s="0" t="s">
-        <v>1523</v>
+        <v>1547</v>
       </c>
       <c r="C622" s="0" t="s">
-        <v>1524</v>
+        <v>1548</v>
       </c>
       <c r="D622" s="0" t="s">
-        <v>1525</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="0" t="s">
-        <v>1526</v>
+        <v>1550</v>
       </c>
       <c r="B623" s="0" t="s">
-        <v>1526</v>
+        <v>1550</v>
       </c>
       <c r="C623" s="0" t="s">
-        <v>1527</v>
+        <v>1551</v>
       </c>
       <c r="D623" s="0" t="s">
-        <v>1528</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="0" t="s">
-        <v>1529</v>
+        <v>1553</v>
       </c>
       <c r="B624" s="0" t="s">
-        <v>1529</v>
+        <v>1553</v>
       </c>
       <c r="C624" s="0" t="s">
-        <v>1530</v>
+        <v>1554</v>
       </c>
       <c r="D624" s="0" t="s">
-        <v>1531</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="0" t="s">
-        <v>1532</v>
+        <v>1556</v>
       </c>
       <c r="B625" s="0" t="s">
-        <v>1532</v>
+        <v>1556</v>
       </c>
       <c r="C625" s="0" t="s">
-        <v>1533</v>
+        <v>1557</v>
       </c>
       <c r="D625" s="0" t="s">
-        <v>1534</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="0" t="s">
-        <v>1535</v>
+        <v>1559</v>
       </c>
       <c r="B626" s="0" t="s">
-        <v>1535</v>
+        <v>1559</v>
       </c>
       <c r="C626" s="0" t="s">
-        <v>1536</v>
+        <v>1560</v>
       </c>
       <c r="D626" s="0" t="s">
-        <v>1537</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="0" t="s">
-        <v>1538</v>
+        <v>1562</v>
       </c>
       <c r="B627" s="0" t="s">
-        <v>1538</v>
+        <v>1562</v>
       </c>
       <c r="C627" s="0" t="s">
-        <v>1539</v>
+        <v>1563</v>
       </c>
       <c r="D627" s="0" t="s">
-        <v>1540</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="0" t="s">
-        <v>1541</v>
+        <v>1565</v>
       </c>
       <c r="B628" s="0" t="s">
-        <v>1541</v>
+        <v>1565</v>
       </c>
       <c r="C628" s="0" t="s">
-        <v>1542</v>
+        <v>1566</v>
       </c>
       <c r="D628" s="0" t="s">
-        <v>1543</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="0" t="s">
-        <v>1544</v>
+        <v>1568</v>
       </c>
       <c r="B629" s="0" t="s">
-        <v>1544</v>
+        <v>1568</v>
       </c>
       <c r="C629" s="0" t="s">
-        <v>1545</v>
+        <v>1569</v>
       </c>
       <c r="D629" s="0" t="s">
-        <v>1546</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="0" t="s">
-        <v>1547</v>
+        <v>1571</v>
       </c>
       <c r="B630" s="0" t="s">
-        <v>1547</v>
+        <v>1571</v>
       </c>
       <c r="C630" s="0" t="s">
-        <v>1548</v>
+        <v>1572</v>
       </c>
       <c r="D630" s="0" t="s">
-        <v>1549</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="0" t="s">
-        <v>1550</v>
+        <v>1574</v>
       </c>
       <c r="B631" s="0" t="s">
-        <v>1550</v>
+        <v>1574</v>
       </c>
       <c r="C631" s="0" t="s">
-        <v>1551</v>
+        <v>1575</v>
       </c>
       <c r="D631" s="0" t="s">
-        <v>1552</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="0" t="s">
-        <v>1553</v>
+        <v>1577</v>
       </c>
       <c r="B632" s="0" t="s">
-        <v>1553</v>
+        <v>1577</v>
       </c>
       <c r="C632" s="0" t="s">
-        <v>1554</v>
+        <v>1578</v>
       </c>
       <c r="D632" s="0" t="s">
-        <v>1555</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="0" t="s">
-        <v>1556</v>
+        <v>1580</v>
       </c>
       <c r="B633" s="0" t="s">
-        <v>1556</v>
+        <v>1580</v>
       </c>
       <c r="C633" s="0" t="s">
-        <v>1557</v>
+        <v>1581</v>
       </c>
       <c r="D633" s="0" t="s">
-        <v>1558</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="0" t="s">
-        <v>1559</v>
+        <v>1583</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>1559</v>
+        <v>1583</v>
       </c>
       <c r="C634" s="0" t="s">
-        <v>1560</v>
+        <v>1584</v>
       </c>
       <c r="D634" s="0" t="s">
-        <v>1561</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="0" t="s">
-        <v>1562</v>
+        <v>1586</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>1562</v>
+        <v>1586</v>
       </c>
       <c r="C635" s="0" t="s">
-        <v>1563</v>
+        <v>1587</v>
       </c>
       <c r="D635" s="0" t="s">
-        <v>1564</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="0" t="s">
-        <v>1565</v>
+        <v>1589</v>
       </c>
       <c r="B636" s="0" t="s">
-        <v>1565</v>
+        <v>1589</v>
       </c>
       <c r="C636" s="0" t="s">
-        <v>1566</v>
+        <v>1590</v>
       </c>
       <c r="D636" s="0" t="s">
-        <v>1567</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="0" t="s">
-        <v>1568</v>
+        <v>1592</v>
       </c>
       <c r="B637" s="0" t="s">
-        <v>1568</v>
+        <v>1592</v>
       </c>
       <c r="C637" s="0" t="s">
-        <v>1569</v>
+        <v>1593</v>
       </c>
       <c r="D637" s="0" t="s">
-        <v>1570</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="0" t="s">
-        <v>1571</v>
+        <v>1595</v>
       </c>
       <c r="B638" s="0" t="s">
-        <v>1571</v>
+        <v>1595</v>
       </c>
       <c r="C638" s="0" t="s">
-        <v>1572</v>
+        <v>1596</v>
       </c>
       <c r="D638" s="0" t="s">
-        <v>1573</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="0" t="s">
-        <v>1574</v>
+        <v>1598</v>
       </c>
       <c r="B639" s="0" t="s">
-        <v>1574</v>
+        <v>1598</v>
       </c>
       <c r="C639" s="0" t="s">
-        <v>1575</v>
+        <v>1599</v>
       </c>
       <c r="D639" s="0" t="s">
-        <v>1576</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="640" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="0" t="s">
-        <v>1577</v>
+        <v>1601</v>
       </c>
       <c r="B640" s="0" t="s">
-        <v>1577</v>
+        <v>1601</v>
       </c>
       <c r="C640" s="0" t="s">
-        <v>1578</v>
+        <v>1602</v>
       </c>
       <c r="D640" s="0" t="s">
-        <v>1579</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="0" t="s">
-        <v>1580</v>
+        <v>1604</v>
       </c>
       <c r="B641" s="0" t="s">
-        <v>1580</v>
+        <v>1604</v>
       </c>
       <c r="C641" s="0" t="s">
-        <v>1581</v>
+        <v>1605</v>
       </c>
       <c r="D641" s="0" t="s">
-        <v>1582</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="0" t="s">
-        <v>1583</v>
+        <v>1607</v>
       </c>
       <c r="B642" s="0" t="s">
-        <v>1583</v>
+        <v>1607</v>
       </c>
       <c r="C642" s="0" t="s">
-        <v>1584</v>
+        <v>1608</v>
       </c>
       <c r="D642" s="0" t="s">
-        <v>1585</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="0" t="s">
-        <v>1586</v>
+        <v>1610</v>
       </c>
       <c r="B643" s="0" t="s">
-        <v>1586</v>
+        <v>1610</v>
       </c>
       <c r="C643" s="0" t="s">
-        <v>1587</v>
+        <v>1611</v>
       </c>
       <c r="D643" s="0" t="s">
-        <v>1588</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="0" t="s">
-        <v>1589</v>
+        <v>1613</v>
       </c>
       <c r="B644" s="0" t="s">
-        <v>1589</v>
+        <v>1613</v>
       </c>
       <c r="C644" s="0" t="s">
-        <v>1590</v>
+        <v>1614</v>
       </c>
       <c r="D644" s="0" t="s">
-        <v>1591</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="0" t="s">
-        <v>1592</v>
+        <v>1616</v>
       </c>
       <c r="B645" s="0" t="s">
-        <v>1592</v>
+        <v>1616</v>
       </c>
       <c r="C645" s="0" t="s">
-        <v>1593</v>
+        <v>1617</v>
       </c>
       <c r="D645" s="0" t="s">
-        <v>1594</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="0" t="s">
-        <v>1595</v>
+        <v>1619</v>
       </c>
       <c r="B646" s="0" t="s">
-        <v>1595</v>
+        <v>1619</v>
       </c>
       <c r="C646" s="0" t="s">
-        <v>1596</v>
+        <v>1620</v>
       </c>
       <c r="D646" s="0" t="s">
-        <v>1597</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="0" t="s">
-        <v>1598</v>
+        <v>1622</v>
       </c>
       <c r="B647" s="0" t="s">
-        <v>1598</v>
+        <v>1622</v>
       </c>
       <c r="C647" s="0" t="s">
-        <v>1599</v>
+        <v>1623</v>
       </c>
       <c r="D647" s="0" t="s">
-        <v>1600</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="0" t="s">
-        <v>1601</v>
+        <v>1625</v>
       </c>
       <c r="B648" s="0" t="s">
-        <v>1601</v>
+        <v>1625</v>
       </c>
       <c r="C648" s="0" t="s">
-        <v>1602</v>
+        <v>1626</v>
       </c>
       <c r="D648" s="0" t="s">
-        <v>1603</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="0" t="s">
-        <v>1604</v>
+        <v>1628</v>
       </c>
       <c r="B649" s="0" t="s">
-        <v>1604</v>
+        <v>1628</v>
       </c>
       <c r="C649" s="0" t="s">
-        <v>1605</v>
+        <v>1629</v>
       </c>
       <c r="D649" s="0" t="s">
-        <v>1606</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="0" t="s">
-        <v>1607</v>
+        <v>1631</v>
       </c>
       <c r="B650" s="0" t="s">
-        <v>1607</v>
+        <v>1631</v>
       </c>
       <c r="C650" s="0" t="s">
-        <v>1608</v>
+        <v>1632</v>
       </c>
       <c r="D650" s="0" t="s">
-        <v>1609</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="0" t="s">
-        <v>1610</v>
+        <v>1634</v>
       </c>
       <c r="B651" s="0" t="s">
-        <v>1610</v>
+        <v>1634</v>
       </c>
       <c r="C651" s="0" t="s">
-        <v>1611</v>
+        <v>1635</v>
       </c>
       <c r="D651" s="0" t="s">
-        <v>1612</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="0" t="s">
-        <v>1613</v>
+        <v>1637</v>
       </c>
       <c r="B652" s="0" t="s">
-        <v>1613</v>
+        <v>1637</v>
       </c>
       <c r="C652" s="0" t="s">
-        <v>1614</v>
+        <v>1638</v>
       </c>
       <c r="D652" s="0" t="s">
-        <v>1615</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="0" t="s">
-        <v>1616</v>
+        <v>1640</v>
       </c>
       <c r="B653" s="0" t="s">
-        <v>1616</v>
+        <v>1640</v>
       </c>
       <c r="C653" s="0" t="s">
-        <v>1617</v>
+        <v>1641</v>
       </c>
       <c r="D653" s="0" t="s">
-        <v>1618</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="0" t="s">
-        <v>1619</v>
+        <v>1643</v>
       </c>
       <c r="B654" s="0" t="s">
-        <v>1619</v>
+        <v>1643</v>
       </c>
       <c r="C654" s="0" t="s">
-        <v>1620</v>
+        <v>1644</v>
       </c>
       <c r="D654" s="0" t="s">
-        <v>1621</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="0" t="s">
-        <v>1622</v>
+        <v>1646</v>
       </c>
       <c r="B655" s="0" t="s">
-        <v>1622</v>
+        <v>1646</v>
       </c>
       <c r="C655" s="0" t="s">
-        <v>1623</v>
+        <v>1647</v>
       </c>
       <c r="D655" s="0" t="s">
-        <v>1624</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="0" t="s">
-        <v>1625</v>
+        <v>1649</v>
       </c>
       <c r="B656" s="0" t="s">
-        <v>1625</v>
+        <v>1649</v>
       </c>
       <c r="C656" s="0" t="s">
-        <v>1626</v>
+        <v>1650</v>
       </c>
       <c r="D656" s="0" t="s">
-        <v>1627</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="0" t="s">
-        <v>1628</v>
+        <v>1652</v>
       </c>
       <c r="B657" s="0" t="s">
-        <v>1628</v>
+        <v>1652</v>
       </c>
       <c r="C657" s="0" t="s">
-        <v>1629</v>
+        <v>1653</v>
       </c>
       <c r="D657" s="0" t="s">
-        <v>1630</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="0" t="s">
-        <v>1631</v>
+        <v>1655</v>
       </c>
       <c r="B658" s="0" t="s">
-        <v>1631</v>
+        <v>1655</v>
       </c>
       <c r="C658" s="0" t="s">
-        <v>1632</v>
+        <v>1656</v>
       </c>
       <c r="D658" s="0" t="s">
-        <v>1633</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="0" t="s">
-        <v>1634</v>
+        <v>1658</v>
       </c>
       <c r="B659" s="0" t="s">
-        <v>1634</v>
+        <v>1658</v>
       </c>
       <c r="C659" s="0" t="s">
-        <v>1635</v>
+        <v>1659</v>
       </c>
       <c r="D659" s="0" t="s">
-        <v>1636</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="0" t="s">
-        <v>1637</v>
+        <v>1661</v>
       </c>
       <c r="B660" s="0" t="s">
-        <v>1637</v>
+        <v>1661</v>
       </c>
       <c r="C660" s="0" t="s">
-        <v>1638</v>
+        <v>1662</v>
       </c>
       <c r="D660" s="0" t="s">
-        <v>1639</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="0" t="s">
-        <v>1640</v>
+        <v>1664</v>
       </c>
       <c r="B661" s="0" t="s">
-        <v>1640</v>
+        <v>1664</v>
       </c>
       <c r="C661" s="0" t="s">
-        <v>1641</v>
+        <v>1665</v>
       </c>
       <c r="D661" s="0" t="s">
-        <v>1640</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="0" t="s">
-        <v>1642</v>
+        <v>1666</v>
       </c>
       <c r="B662" s="0" t="s">
-        <v>1642</v>
+        <v>1666</v>
       </c>
       <c r="C662" s="0" t="s">
-        <v>1643</v>
+        <v>1667</v>
       </c>
       <c r="D662" s="0" t="s">
-        <v>1644</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="0" t="s">
-        <v>1645</v>
+        <v>1669</v>
       </c>
       <c r="B663" s="0" t="s">
-        <v>1645</v>
+        <v>1669</v>
       </c>
       <c r="C663" s="0" t="s">
-        <v>1646</v>
+        <v>1670</v>
       </c>
       <c r="D663" s="0" t="s">
-        <v>1647</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="0" t="s">
-        <v>1648</v>
+        <v>1672</v>
       </c>
       <c r="B664" s="0" t="s">
-        <v>1648</v>
+        <v>1672</v>
       </c>
       <c r="C664" s="0" t="s">
-        <v>1649</v>
+        <v>1673</v>
       </c>
       <c r="D664" s="0" t="s">
-        <v>1650</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="0" t="s">
-        <v>1651</v>
+        <v>1675</v>
       </c>
       <c r="B665" s="0" t="s">
-        <v>1651</v>
+        <v>1675</v>
       </c>
       <c r="C665" s="0" t="s">
-        <v>1652</v>
+        <v>1676</v>
       </c>
       <c r="D665" s="0" t="s">
-        <v>1653</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="0" t="s">
-        <v>1654</v>
+        <v>1678</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>1654</v>
+        <v>1678</v>
       </c>
       <c r="C666" s="2" t="s">
-        <v>1655</v>
+        <v>1679</v>
       </c>
       <c r="D666" s="0" t="s">
-        <v>1656</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="2" t="s">
-        <v>1657</v>
+        <v>1681</v>
       </c>
       <c r="B667" s="0" t="s">
-        <v>1657</v>
+        <v>1681</v>
       </c>
       <c r="C667" s="0" t="s">
-        <v>1658</v>
+        <v>1682</v>
       </c>
       <c r="D667" s="0" t="s">
-        <v>1659</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="0" t="s">
-        <v>1660</v>
+        <v>1684</v>
       </c>
       <c r="B668" s="0" t="s">
-        <v>1660</v>
+        <v>1684</v>
       </c>
       <c r="C668" s="0" t="s">
-        <v>1661</v>
+        <v>1685</v>
       </c>
       <c r="D668" s="0" t="s">
-        <v>1662</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="0" t="s">
-        <v>1663</v>
+        <v>1687</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>1663</v>
+        <v>1687</v>
       </c>
       <c r="C669" s="2" t="s">
-        <v>1664</v>
+        <v>1688</v>
       </c>
       <c r="D669" s="0" t="s">
-        <v>1665</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="2" t="s">
-        <v>1666</v>
+        <v>1690</v>
       </c>
       <c r="B670" s="0" t="s">
-        <v>1666</v>
+        <v>1690</v>
       </c>
       <c r="C670" s="0" t="s">
-        <v>1667</v>
+        <v>1691</v>
       </c>
       <c r="D670" s="0" t="s">
-        <v>1668</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="0" t="s">
-        <v>1669</v>
+        <v>1693</v>
       </c>
       <c r="B671" s="0" t="s">
-        <v>1669</v>
+        <v>1693</v>
       </c>
       <c r="C671" s="0" t="s">
-        <v>1670</v>
+        <v>1694</v>
       </c>
       <c r="D671" s="0" t="s">
-        <v>1669</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="0" t="s">
-        <v>1671</v>
+        <v>1695</v>
       </c>
       <c r="B672" s="0" t="s">
-        <v>1672</v>
+        <v>1696</v>
+      </c>
+      <c r="D672" s="0" t="s">
+        <v>1697</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="0" t="s">
-        <v>1673</v>
+        <v>1698</v>
       </c>
       <c r="B673" s="0" t="s">
-        <v>1674</v>
+        <v>1699</v>
+      </c>
+      <c r="D673" s="0" t="s">
+        <v>1700</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="0" t="s">
-        <v>1675</v>
+        <v>1701</v>
       </c>
       <c r="B674" s="0" t="s">
-        <v>1676</v>
+        <v>1702</v>
+      </c>
+      <c r="D674" s="0" t="s">
+        <v>1703</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A678" s="0" t="s">
+        <v>1704</v>
+      </c>
+    </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="0" t="s">
-        <v>1677</v>
+        <v>1705</v>
+      </c>
+      <c r="B679" s="0" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C679" s="0" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D679" s="0" t="s">
+        <v>1707</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="0" t="s">
-        <v>1678</v>
+        <v>1708</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1678</v>
+        <v>1708</v>
       </c>
       <c r="C680" s="0" t="s">
-        <v>1679</v>
+        <v>1709</v>
       </c>
       <c r="D680" s="0" t="s">
-        <v>1680</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="0" t="s">
-        <v>1681</v>
+        <v>1711</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>1681</v>
+        <v>1711</v>
       </c>
       <c r="C681" s="0" t="s">
-        <v>1682</v>
+        <v>1712</v>
       </c>
       <c r="D681" s="0" t="s">
-        <v>1683</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="0" t="s">
-        <v>1684</v>
+        <v>1714</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>1684</v>
+        <v>1714</v>
       </c>
       <c r="C682" s="0" t="s">
-        <v>1685</v>
+        <v>1715</v>
       </c>
       <c r="D682" s="0" t="s">
-        <v>1686</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="0" t="s">
-        <v>1687</v>
+        <v>1717</v>
       </c>
       <c r="B683" s="0" t="s">
-        <v>1687</v>
+        <v>1717</v>
       </c>
       <c r="C683" s="0" t="s">
-        <v>1688</v>
+        <v>1718</v>
       </c>
       <c r="D683" s="0" t="s">
-        <v>1689</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="0" t="s">
-        <v>1690</v>
+        <v>1720</v>
       </c>
       <c r="B684" s="0" t="s">
-        <v>1690</v>
+        <v>1720</v>
       </c>
       <c r="C684" s="0" t="s">
-        <v>1691</v>
+        <v>1721</v>
       </c>
       <c r="D684" s="0" t="s">
-        <v>1692</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="0" t="s">
-        <v>1693</v>
+        <v>1723</v>
       </c>
       <c r="B685" s="0" t="s">
-        <v>1693</v>
+        <v>1723</v>
       </c>
       <c r="C685" s="0" t="s">
-        <v>1694</v>
+        <v>1724</v>
       </c>
       <c r="D685" s="0" t="s">
-        <v>1695</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="0" t="s">
-        <v>1696</v>
+        <v>1726</v>
       </c>
       <c r="B686" s="0" t="s">
-        <v>1696</v>
+        <v>1726</v>
       </c>
       <c r="C686" s="0" t="s">
-        <v>1697</v>
+        <v>1727</v>
       </c>
       <c r="D686" s="0" t="s">
-        <v>1698</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="0" t="s">
-        <v>1699</v>
+        <v>1729</v>
       </c>
       <c r="B687" s="0" t="s">
-        <v>1699</v>
+        <v>1729</v>
       </c>
       <c r="C687" s="0" t="s">
-        <v>1700</v>
+        <v>1730</v>
       </c>
       <c r="D687" s="0" t="s">
-        <v>1701</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="0" t="s">
-        <v>1702</v>
+        <v>1732</v>
       </c>
       <c r="B688" s="0" t="s">
-        <v>1702</v>
+        <v>1732</v>
       </c>
       <c r="C688" s="0" t="s">
-        <v>1703</v>
+        <v>1733</v>
       </c>
       <c r="D688" s="0" t="s">
-        <v>1704</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="0" t="s">
-        <v>1705</v>
+        <v>1735</v>
       </c>
       <c r="B689" s="0" t="s">
-        <v>1705</v>
+        <v>1735</v>
       </c>
       <c r="C689" s="0" t="s">
-        <v>1706</v>
+        <v>1736</v>
       </c>
       <c r="D689" s="0" t="s">
-        <v>1707</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="0" t="s">
-        <v>1708</v>
+        <v>1738</v>
       </c>
       <c r="B690" s="0" t="s">
-        <v>1708</v>
+        <v>1739</v>
       </c>
       <c r="C690" s="0" t="s">
-        <v>1709</v>
+        <v>1740</v>
       </c>
       <c r="D690" s="0" t="s">
-        <v>1710</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="0" t="s">
-        <v>1711</v>
+        <v>1742</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>1712</v>
+        <v>1742</v>
       </c>
       <c r="C691" s="0" t="s">
-        <v>1713</v>
+        <v>1743</v>
       </c>
       <c r="D691" s="0" t="s">
-        <v>1714</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="0" t="s">
-        <v>1715</v>
+        <v>1745</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>1715</v>
+        <v>1745</v>
       </c>
       <c r="C692" s="0" t="s">
-        <v>1716</v>
+        <v>1746</v>
       </c>
       <c r="D692" s="0" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="0" t="s">
-        <v>1718</v>
+        <v>1748</v>
       </c>
       <c r="B693" s="0" t="s">
-        <v>1718</v>
+        <v>1748</v>
       </c>
       <c r="C693" s="0" t="s">
-        <v>1719</v>
-      </c>
-      <c r="D693" s="0" t="s">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="0" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B694" s="0" t="s">
-        <v>1721</v>
-      </c>
-      <c r="C694" s="0" t="s">
-        <v>1722</v>
-      </c>
-      <c r="D694" s="3" t="s">
-        <v>1723</v>
-      </c>
-    </row>
+        <v>1749</v>
+      </c>
+      <c r="D693" s="1" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>